<commit_message>
tweaking unit tests; smb file server; web filter unittests
</commit_message>
<xml_diff>
--- a/docs/TOGAF/Artifacts/Catalogs/Preliminary/McSOC Principles Catalog.xlsx
+++ b/docs/TOGAF/Artifacts/Catalogs/Preliminary/McSOC Principles Catalog.xlsx
@@ -189,7 +189,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="207">
   <si>
     <t>Architecture Principles</t>
   </si>
@@ -233,7 +233,7 @@
     <t>“Say what you do”</t>
   </si>
   <si>
-    <t>Full documentation of capabilities and limitations of McSOC. </t>
+    <t>Full documentation of capabilities and limitations of McSOC.</t>
   </si>
   <si>
     <t>PRN_ARC_02</t>
@@ -724,13 +724,37 @@
     <t>PRN_SE_01</t>
   </si>
   <si>
+    <t>Defense-in-depth: Virtual</t>
+  </si>
+  <si>
+    <t>In a traditional architecture, this would be the physical layer. In this virtualized environment, it is the virtual server itself.</t>
+  </si>
+  <si>
     <t>PRN_SE_02</t>
   </si>
   <si>
+    <t>Defense-in-depth: Network</t>
+  </si>
+  <si>
+    <t>Routing, Network Firewalls, End point Firewalls, encryption, No unnecessary services</t>
+  </si>
+  <si>
     <t>PRN_SE_03</t>
   </si>
   <si>
+    <t>Defense-in-depth: Host</t>
+  </si>
+  <si>
+    <t>Secure configuration and software patching</t>
+  </si>
+  <si>
     <t>PRN_SE_04</t>
+  </si>
+  <si>
+    <t>Defense-in-depth: Application</t>
+  </si>
+  <si>
+    <t>Secure configuration, role-based access control, encryption</t>
   </si>
   <si>
     <t>PRN_SE_05</t>
@@ -1067,7 +1091,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -2350,7 +2374,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" s="4" customFormat="true" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" s="4" customFormat="true" ht="40.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
         <v>103</v>
       </c>
@@ -2373,7 +2397,7 @@
       <c r="J3" s="9"/>
       <c r="K3" s="9"/>
     </row>
-    <row r="4" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="34.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
         <v>108</v>
       </c>
@@ -3083,7 +3107,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -3144,12 +3168,16 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" s="4" customFormat="true" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" s="4" customFormat="true" ht="34.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
+      <c r="B3" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>160</v>
+      </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
@@ -3159,12 +3187,16 @@
       <c r="J3" s="9"/>
       <c r="K3" s="9"/>
     </row>
-    <row r="4" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
+        <v>161</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>163</v>
+      </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
@@ -3174,12 +3206,16 @@
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
     </row>
-    <row r="5" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="10"/>
+        <v>164</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>166</v>
+      </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
@@ -3189,12 +3225,16 @@
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
     </row>
-    <row r="6" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="10"/>
+        <v>167</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>169</v>
+      </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
@@ -3206,7 +3246,7 @@
     </row>
     <row r="7" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="10"/>
@@ -3221,7 +3261,7 @@
     </row>
     <row r="8" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="10"/>
@@ -3236,7 +3276,7 @@
     </row>
     <row r="9" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="10"/>
@@ -3251,7 +3291,7 @@
     </row>
     <row r="10" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="10"/>
@@ -3266,7 +3306,7 @@
     </row>
     <row r="11" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="10"/>
@@ -3281,7 +3321,7 @@
     </row>
     <row r="12" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="11"/>
@@ -3296,7 +3336,7 @@
     </row>
     <row r="13" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="12"/>
@@ -3311,7 +3351,7 @@
     </row>
     <row r="14" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -3326,7 +3366,7 @@
     </row>
     <row r="15" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -3341,7 +3381,7 @@
     </row>
     <row r="16" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -3356,7 +3396,7 @@
     </row>
     <row r="17" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -3371,7 +3411,7 @@
     </row>
     <row r="18" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -3386,7 +3426,7 @@
     </row>
     <row r="19" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -3401,7 +3441,7 @@
     </row>
     <row r="20" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="8" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -3416,7 +3456,7 @@
     </row>
     <row r="21" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="8" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -3431,7 +3471,7 @@
     </row>
     <row r="22" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -3486,7 +3526,7 @@
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -3530,7 +3570,7 @@
     </row>
     <row r="3" s="4" customFormat="true" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -3545,7 +3585,7 @@
     </row>
     <row r="4" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -3560,7 +3600,7 @@
     </row>
     <row r="5" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="10"/>
@@ -3575,7 +3615,7 @@
     </row>
     <row r="6" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="10"/>
@@ -3590,7 +3630,7 @@
     </row>
     <row r="7" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="10"/>
@@ -3605,7 +3645,7 @@
     </row>
     <row r="8" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="10"/>
@@ -3620,7 +3660,7 @@
     </row>
     <row r="9" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="10"/>
@@ -3635,7 +3675,7 @@
     </row>
     <row r="10" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="10"/>
@@ -3650,7 +3690,7 @@
     </row>
     <row r="11" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="10"/>
@@ -3665,7 +3705,7 @@
     </row>
     <row r="12" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="11"/>
@@ -3680,7 +3720,7 @@
     </row>
     <row r="13" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="12"/>
@@ -3695,7 +3735,7 @@
     </row>
     <row r="14" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -3710,7 +3750,7 @@
     </row>
     <row r="15" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -3725,7 +3765,7 @@
     </row>
     <row r="16" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -3740,7 +3780,7 @@
     </row>
     <row r="17" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -3755,7 +3795,7 @@
     </row>
     <row r="18" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -3770,7 +3810,7 @@
     </row>
     <row r="19" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -3785,7 +3825,7 @@
     </row>
     <row r="20" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="8" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -3800,7 +3840,7 @@
     </row>
     <row r="21" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="8" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -3815,7 +3855,7 @@
     </row>
     <row r="22" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>

</xml_diff>